<commit_message>
Add slides on association
</commit_message>
<xml_diff>
--- a/teaching_plan.xlsx
+++ b/teaching_plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acobo\Documents\MEGA\ACC\Docencia\Clinic CDB\Edition 2\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acobo\Documents\MEGA\ACC\Docencia\Clinic CDB\Edition 2\CDB_ed2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237EEA0A-5FFC-40B9-B7F1-C98D78DF046C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D490E-EAC5-437E-8FD7-324CF6135E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="2865" windowWidth="21855" windowHeight="12555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sessions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
   <si>
     <t>session</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t>Reporting with Rmarkdown (pending)</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>4_0_association</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085B7C2F-2716-49CF-AF47-77170B7E49A7}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,13 +1515,13 @@
         <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1529,32 +1535,32 @@
         <v>41</v>
       </c>
       <c r="D34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
         <v>84</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>9</v>
-      </c>
-      <c r="B36" s="3">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1569,32 +1575,32 @@
         <v>41</v>
       </c>
       <c r="D37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>9</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" t="s">
         <v>86</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>10</v>
-      </c>
-      <c r="B39" s="3">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1609,33 +1615,33 @@
         <v>41</v>
       </c>
       <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>10</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
         <v>94</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>93</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>11</v>
-      </c>
-      <c r="B42" s="3">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>58</v>
+      <c r="F41" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1649,13 +1655,13 @@
         <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1669,32 +1675,32 @@
         <v>28</v>
       </c>
       <c r="D44" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>11</v>
+      </c>
+      <c r="B45" s="3">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
         <v>102</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>98</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>12</v>
-      </c>
-      <c r="B46" s="3">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" t="s">
-        <v>99</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1709,10 +1715,10 @@
         <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E47" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>59</v>
@@ -1729,32 +1735,32 @@
         <v>28</v>
       </c>
       <c r="D48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
         <v>105</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>13</v>
-      </c>
-      <c r="B50" s="3">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1769,38 +1775,38 @@
         <v>28</v>
       </c>
       <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>13</v>
+      </c>
+      <c r="B52" s="3">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
         <v>106</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>14</v>
-      </c>
-      <c r="B53" s="3">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" t="s">
-        <v>113</v>
-      </c>
-      <c r="F53" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" s="3">
         <v>6</v>
@@ -1809,18 +1815,18 @@
         <v>116</v>
       </c>
       <c r="D54" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" s="3">
         <v>6</v>
@@ -1829,12 +1835,32 @@
         <v>116</v>
       </c>
       <c r="D55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>16</v>
+      </c>
+      <c r="B56" s="3">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" t="s">
         <v>118</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>114</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rmarkdown slides and exes
</commit_message>
<xml_diff>
--- a/teaching_plan.xlsx
+++ b/teaching_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acobo\Documents\MEGA\ACC\Docencia\Clinic CDB\Edition 2\CDB_ed2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D490E-EAC5-437E-8FD7-324CF6135E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9B3296-6922-46A9-A4E6-C7912749DA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
   <si>
     <t>session</t>
   </si>
@@ -382,13 +382,19 @@
     <t>6_2_funs</t>
   </si>
   <si>
-    <t>Reporting with Rmarkdown (pending)</t>
-  </si>
-  <si>
     <t>Association</t>
   </si>
   <si>
     <t>4_0_association</t>
+  </si>
+  <si>
+    <t>Rmarkdown</t>
+  </si>
+  <si>
+    <t>More Rmarkdown</t>
+  </si>
+  <si>
+    <t>6_4_more_rmarkdown</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085B7C2F-2716-49CF-AF47-77170B7E49A7}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,10 +1521,10 @@
         <v>41</v>
       </c>
       <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
         <v>119</v>
-      </c>
-      <c r="E33" t="s">
-        <v>120</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>58</v>
@@ -1855,13 +1861,33 @@
         <v>116</v>
       </c>
       <c r="D56" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E56" t="s">
         <v>114</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>16</v>
+      </c>
+      <c r="B57" s="3">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" t="s">
+        <v>121</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exercise added to 6.2 funs
</commit_message>
<xml_diff>
--- a/teaching_plan.xlsx
+++ b/teaching_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acobo\Documents\MEGA\ACC\Docencia\Clinic CDB\Edition 2\CDB_ed2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34960607-D66E-43E6-94A0-3353BC7BDE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C153869B-8F0A-4908-92DA-2E27A97700B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,7 +1847,7 @@
         <v>116</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>